<commit_message>
I exported the data to test progenitor separation using Adam Goldstein's hypothesis, but with known progenitors added
</commit_message>
<xml_diff>
--- a/fermi_known_progenitors_list.xlsx
+++ b/fermi_known_progenitors_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nnuessle/Documents/Work/burst_matching_algorithm/actual_paper/prompt-and-afterglow-matching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ED9CDA-A898-E946-A5E4-AE09E0A5109F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01335580-3009-EF47-A638-91A3E63E130F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="1400" windowWidth="30420" windowHeight="16940" activeTab="1" xr2:uid="{415A39E4-12E1-0D46-96F2-16C855D612ED}"/>
+    <workbookView xWindow="220" yWindow="1520" windowWidth="30420" windowHeight="16940" activeTab="1" xr2:uid="{415A39E4-12E1-0D46-96F2-16C855D612ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="2" r:id="rId1"/>
@@ -2367,10 +2367,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B77214D-A0D5-7B44-A3B1-D5FB25B073F0}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60:B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3596,8 +3596,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="26" t="s">
+    <row r="46" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="27" t="s">
         <v>37</v>
       </c>
       <c r="B46" s="15" t="s">
@@ -3627,26 +3627,26 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="26"/>
-      <c r="B47" s="2" t="s">
-        <v>22</v>
+      <c r="B47" t="s">
+        <v>173</v>
       </c>
       <c r="C47" t="s">
-        <v>144</v>
-      </c>
-      <c r="D47" t="s">
-        <v>140</v>
-      </c>
-      <c r="E47" t="s">
-        <v>140</v>
-      </c>
-      <c r="F47" t="s">
-        <v>141</v>
-      </c>
-      <c r="G47" t="s">
-        <v>141</v>
-      </c>
-      <c r="H47" t="s">
-        <v>140</v>
+        <v>164</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>141</v>
       </c>
       <c r="I47" t="s">
         <v>141</v>
@@ -3654,11 +3654,11 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="26"/>
-      <c r="B48" s="3" t="s">
-        <v>25</v>
+      <c r="B48" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D48" t="s">
         <v>140</v>
@@ -3667,52 +3667,52 @@
         <v>140</v>
       </c>
       <c r="F48" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G48" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H48" t="s">
         <v>140</v>
       </c>
       <c r="I48" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="26"/>
-      <c r="B49" s="1" t="s">
-        <v>26</v>
+      <c r="B49" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D49" t="s">
         <v>140</v>
       </c>
       <c r="E49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F49" t="s">
         <v>140</v>
       </c>
       <c r="G49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="26"/>
-      <c r="B50" s="2" t="s">
-        <v>23</v>
+      <c r="B50" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D50" t="s">
         <v>140</v>
@@ -3721,7 +3721,7 @@
         <v>141</v>
       </c>
       <c r="F50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G50" t="s">
         <v>141</v>
@@ -3735,14 +3735,14 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="26"/>
-      <c r="B51" s="3" t="s">
-        <v>27</v>
+      <c r="B51" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E51" t="s">
         <v>141</v>
@@ -3762,239 +3762,239 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="26"/>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" t="s">
+        <v>141</v>
+      </c>
+      <c r="F52" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52" t="s">
+        <v>141</v>
+      </c>
+      <c r="H52" t="s">
+        <v>141</v>
+      </c>
+      <c r="I52" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="26"/>
+      <c r="B53" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>149</v>
       </c>
-      <c r="D52" t="s">
-        <v>140</v>
-      </c>
-      <c r="E52" t="s">
-        <v>140</v>
-      </c>
-      <c r="F52" t="s">
-        <v>141</v>
-      </c>
-      <c r="G52" t="s">
-        <v>141</v>
-      </c>
-      <c r="H52" t="s">
-        <v>141</v>
-      </c>
-      <c r="I52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="27" t="s">
+      <c r="D53" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" t="s">
+        <v>140</v>
+      </c>
+      <c r="F53" t="s">
+        <v>141</v>
+      </c>
+      <c r="G53" t="s">
+        <v>141</v>
+      </c>
+      <c r="H53" t="s">
+        <v>141</v>
+      </c>
+      <c r="I53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B54" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C54" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="D53" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="G53" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="I53" s="13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="26"/>
-      <c r="B54" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" t="s">
-        <v>151</v>
-      </c>
-      <c r="D54" t="s">
-        <v>140</v>
-      </c>
-      <c r="E54" t="s">
-        <v>141</v>
-      </c>
-      <c r="F54" t="s">
-        <v>141</v>
-      </c>
-      <c r="G54" t="s">
-        <v>141</v>
-      </c>
-      <c r="H54" t="s">
-        <v>141</v>
-      </c>
-      <c r="I54" t="s">
+      <c r="D54" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="I54" s="13" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="26"/>
-      <c r="B55" s="3" t="s">
-        <v>31</v>
+      <c r="B55" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="G55" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="H55" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="I55" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" t="s">
+        <v>141</v>
+      </c>
+      <c r="H55" t="s">
+        <v>141</v>
+      </c>
+      <c r="I55" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="26"/>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="H56" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I56" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="26"/>
+      <c r="B57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>153</v>
       </c>
-      <c r="D56" t="s">
-        <v>140</v>
-      </c>
-      <c r="E56" t="s">
-        <v>140</v>
-      </c>
-      <c r="F56" t="s">
-        <v>141</v>
-      </c>
-      <c r="G56" t="s">
-        <v>141</v>
-      </c>
-      <c r="H56" t="s">
-        <v>141</v>
-      </c>
-      <c r="I56" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="28"/>
-      <c r="B57" s="17" t="s">
+      <c r="D57" t="s">
+        <v>140</v>
+      </c>
+      <c r="E57" t="s">
+        <v>140</v>
+      </c>
+      <c r="F57" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" t="s">
+        <v>141</v>
+      </c>
+      <c r="H57" t="s">
+        <v>141</v>
+      </c>
+      <c r="I57" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="28"/>
+      <c r="B58" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C58" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D57" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F57" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="H57" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="I57" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
+      <c r="D58" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G58" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="H58" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B59" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C59" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D58" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="H58" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="I58" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="27" t="s">
+      <c r="D59" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="H59" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="I59" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>168</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>159</v>
       </c>
-      <c r="D59" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G59" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="H59" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="I59" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="26"/>
-      <c r="B60" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" t="s">
-        <v>160</v>
-      </c>
       <c r="D60" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E60" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F60" s="20" t="s">
         <v>141</v>
@@ -4003,7 +4003,7 @@
         <v>141</v>
       </c>
       <c r="H60" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I60" t="s">
         <v>141</v>
@@ -4012,13 +4012,13 @@
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="26"/>
       <c r="B61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C61" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E61" s="20" t="s">
         <v>141</v>
@@ -4039,10 +4039,10 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="26"/>
       <c r="B62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>140</v>
@@ -4057,7 +4057,7 @@
         <v>141</v>
       </c>
       <c r="H62" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I62" t="s">
         <v>141</v>
@@ -4066,16 +4066,16 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="26"/>
       <c r="B63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D63" s="20" t="s">
         <v>140</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F63" s="20" t="s">
         <v>141</v>
@@ -4084,7 +4084,7 @@
         <v>141</v>
       </c>
       <c r="H63" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I63" t="s">
         <v>141</v>
@@ -4092,17 +4092,17 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="26"/>
-      <c r="B64" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C64" s="22" t="s">
-        <v>164</v>
+      <c r="B64" t="s">
+        <v>172</v>
+      </c>
+      <c r="C64" t="s">
+        <v>163</v>
       </c>
       <c r="D64" s="20" t="s">
         <v>140</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F64" s="20" t="s">
         <v>141</v>
@@ -4111,7 +4111,7 @@
         <v>141</v>
       </c>
       <c r="H64" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I64" t="s">
         <v>141</v>
@@ -4129,19 +4129,19 @@
         <v>140</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F65" s="20" t="s">
         <v>140</v>
       </c>
       <c r="G65" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H65" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -4156,7 +4156,7 @@
         <v>140</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F66" s="20" t="s">
         <v>141</v>
@@ -4183,7 +4183,7 @@
         <v>140</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F67" s="20" t="s">
         <v>141</v>
@@ -4197,13 +4197,16 @@
       <c r="I67" t="s">
         <v>141</v>
       </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A3:A44"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A60:A68"/>
+    <mergeCell ref="A46:A53"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:I1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>